<commit_message>
don't check that the server rejects commands to add status codes that the object already has - or that it rejects commands to remove status codes that it doesn't have.
</commit_message>
<xml_diff>
--- a/data/epp-16-status-data.xlsx
+++ b/data/epp-16-status-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6076A8EC-9F51-6E48-A491-E11FA8F83C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F198E4-DFD7-7646-B2DB-533DF63C7196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="16860" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="34">
   <si>
     <t>errorCode</t>
   </si>
@@ -381,8 +381,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:E41" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="B7:E41" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:E32" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="B7:E32" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -715,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
-  <dimension ref="B2:H41"/>
+  <dimension ref="B2:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:E6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -825,22 +825,23 @@
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>15</v>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H11"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
@@ -854,14 +855,14 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>16</v>
+      <c r="C13" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13"/>
     </row>
@@ -870,7 +871,7 @@
         <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>2</v>
@@ -884,8 +885,8 @@
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>26</v>
+      <c r="C15" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>1</v>
@@ -897,10 +898,10 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>2</v>
@@ -915,13 +916,13 @@
         <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="H17"/>
     </row>
@@ -930,67 +931,63 @@
         <v>10</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H18"/>
+        <v>28</v>
+      </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19"/>
+        <v>28</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H20"/>
+        <v>28</v>
+      </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21"/>
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>1</v>
@@ -998,14 +995,13 @@
       <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H22"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>1</v>
@@ -1019,7 +1015,7 @@
         <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>1</v>
@@ -1033,7 +1029,7 @@
         <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>1</v>
@@ -1047,7 +1043,7 @@
         <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>1</v>
@@ -1061,7 +1057,7 @@
         <v>10</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>1</v>
@@ -1072,63 +1068,63 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>24</v>
@@ -1137,138 +1133,12 @@
         <v>1</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H13:H24">
-    <sortCondition ref="H13:H24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H12:H19">
+    <sortCondition ref="H12:H19"/>
   </sortState>
   <mergeCells count="5">
     <mergeCell ref="B2:E2"/>

</xml_diff>